<commit_message>
añadido respuesta en amplitud y fase
</commit_message>
<xml_diff>
--- a/piTankGo.xlsx
+++ b/piTankGo.xlsx
@@ -1,11 +1,11 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="21425"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="21601"/>
   <workbookPr filterPrivacy="1"/>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{F27A20C2-94A3-4396-A401-9550F1DAE905}" xr6:coauthVersionLast="43" xr6:coauthVersionMax="43" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{F9EC5704-65D0-4D3D-84AF-1F168E3813DA}" xr6:coauthVersionLast="43" xr6:coauthVersionMax="43" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-98" yWindow="-98" windowWidth="22695" windowHeight="14595" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-98" yWindow="-98" windowWidth="22695" windowHeight="14595" activeTab="2" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Paso AltoF" sheetId="1" r:id="rId1"/>
@@ -28,7 +28,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="10" uniqueCount="7">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="12" uniqueCount="9">
   <si>
     <t>Entrada (V)</t>
   </si>
@@ -49,6 +49,12 @@
   </si>
   <si>
     <t>Fase</t>
+  </si>
+  <si>
+    <t>A</t>
+  </si>
+  <si>
+    <t>C</t>
   </si>
 </sst>
 </file>
@@ -574,7 +580,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{CB35D0F8-3512-4C7B-9C0D-73C46B06FF73}">
   <dimension ref="A1"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0"/>
+    <sheetView workbookViewId="0"/>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.25" x14ac:dyDescent="0.45"/>
   <sheetData/>
@@ -584,10 +590,10 @@
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{04BF7135-059E-4F20-807E-C5ECB98BA8C1}">
-  <dimension ref="A1:E12"/>
+  <dimension ref="A1:G21"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="D2" sqref="D2"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="B27" sqref="B27"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.25" x14ac:dyDescent="0.45"/>
@@ -595,7 +601,7 @@
     <col min="2" max="2" width="19.53125" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:5" x14ac:dyDescent="0.45">
+    <row r="1" spans="1:7" x14ac:dyDescent="0.45">
       <c r="A1" t="s">
         <v>3</v>
       </c>
@@ -611,168 +617,387 @@
       <c r="E1" t="s">
         <v>6</v>
       </c>
-    </row>
-    <row r="2" spans="1:5" x14ac:dyDescent="0.45">
+      <c r="F1" t="s">
+        <v>7</v>
+      </c>
+      <c r="G1" t="s">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="2" spans="1:7" x14ac:dyDescent="0.45">
       <c r="A2">
-        <v>3.3</v>
+        <v>3.16</v>
       </c>
       <c r="B2">
-        <v>18</v>
+        <v>5</v>
       </c>
       <c r="C2">
-        <v>3.3</v>
+        <v>3.16</v>
       </c>
       <c r="D2">
-        <v>0</v>
+        <v>0.19400000000000001</v>
       </c>
       <c r="E2">
         <f>D2*B2*360</f>
-        <v>0</v>
-      </c>
-    </row>
-    <row r="3" spans="1:5" x14ac:dyDescent="0.45">
+        <v>349.2</v>
+      </c>
+    </row>
+    <row r="3" spans="1:7" x14ac:dyDescent="0.45">
+      <c r="A3">
+        <v>3.16</v>
+      </c>
       <c r="B3">
-        <v>180</v>
+        <v>10</v>
       </c>
       <c r="C3">
-        <v>3.3</v>
-      </c>
-      <c r="D3" s="1"/>
+        <v>3.16</v>
+      </c>
+      <c r="D3" s="1">
+        <v>9.8400000000000001E-2</v>
+      </c>
       <c r="E3">
         <f t="shared" ref="E3:E10" si="0">D3*B3*360</f>
+        <v>354.24</v>
+      </c>
+    </row>
+    <row r="4" spans="1:7" x14ac:dyDescent="0.45">
+      <c r="A4">
+        <v>3.16</v>
+      </c>
+      <c r="B4">
+        <v>20</v>
+      </c>
+      <c r="C4">
+        <v>3.16</v>
+      </c>
+      <c r="D4" s="1">
+        <v>0.05</v>
+      </c>
+      <c r="E4">
+        <f t="shared" si="0"/>
+        <v>360</v>
+      </c>
+    </row>
+    <row r="5" spans="1:7" x14ac:dyDescent="0.45">
+      <c r="A5">
+        <v>3.16</v>
+      </c>
+      <c r="B5">
+        <v>40</v>
+      </c>
+      <c r="C5">
+        <v>3.16</v>
+      </c>
+      <c r="D5" s="1">
         <v>0</v>
       </c>
-    </row>
-    <row r="4" spans="1:5" x14ac:dyDescent="0.45">
-      <c r="B4">
-        <v>1800</v>
-      </c>
-      <c r="C4">
-        <v>3.2</v>
-      </c>
-      <c r="D4" s="1">
-        <v>1.7E-5</v>
-      </c>
-      <c r="E4">
-        <f t="shared" si="0"/>
-        <v>11.016</v>
-      </c>
-    </row>
-    <row r="5" spans="1:5" x14ac:dyDescent="0.45">
-      <c r="B5">
-        <v>5000</v>
-      </c>
-      <c r="C5">
-        <v>3</v>
-      </c>
-      <c r="D5" s="1">
-        <v>1.56E-5</v>
-      </c>
       <c r="E5">
         <f t="shared" si="0"/>
-        <v>28.08</v>
-      </c>
-    </row>
-    <row r="6" spans="1:5" x14ac:dyDescent="0.45">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="6" spans="1:7" x14ac:dyDescent="0.45">
+      <c r="A6">
+        <v>3.16</v>
+      </c>
       <c r="B6">
-        <v>10000</v>
+        <v>80.599999999999994</v>
       </c>
       <c r="C6">
-        <v>2.4</v>
+        <v>3.16</v>
       </c>
       <c r="D6" s="1">
-        <v>1.3200000000000001E-5</v>
+        <v>0</v>
       </c>
       <c r="E6">
         <f t="shared" si="0"/>
-        <v>47.52</v>
-      </c>
-    </row>
-    <row r="7" spans="1:5" x14ac:dyDescent="0.45">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="7" spans="1:7" x14ac:dyDescent="0.45">
+      <c r="A7">
+        <v>3.16</v>
+      </c>
       <c r="B7">
-        <v>15000</v>
+        <v>800</v>
       </c>
       <c r="C7">
-        <v>1.8</v>
+        <v>3.12</v>
       </c>
       <c r="D7" s="1">
         <v>1.2E-5</v>
       </c>
       <c r="E7">
         <f t="shared" si="0"/>
-        <v>64.8</v>
-      </c>
-    </row>
-    <row r="8" spans="1:5" x14ac:dyDescent="0.45">
+        <v>3.4560000000000004</v>
+      </c>
+    </row>
+    <row r="8" spans="1:7" x14ac:dyDescent="0.45">
+      <c r="A8">
+        <v>3.16</v>
+      </c>
       <c r="B8">
-        <v>18000</v>
+        <v>1600</v>
       </c>
       <c r="C8">
+        <v>3.12</v>
+      </c>
+      <c r="D8" s="1">
+        <v>1.5999999999999999E-5</v>
+      </c>
+      <c r="E8">
+        <f t="shared" si="0"/>
+        <v>9.2159999999999993</v>
+      </c>
+    </row>
+    <row r="9" spans="1:7" x14ac:dyDescent="0.45">
+      <c r="A9">
+        <v>3.16</v>
+      </c>
+      <c r="B9">
+        <v>3200</v>
+      </c>
+      <c r="C9">
+        <v>3.06</v>
+      </c>
+      <c r="D9" s="1">
+        <v>1.7E-5</v>
+      </c>
+      <c r="E9">
+        <f t="shared" si="0"/>
+        <v>19.584</v>
+      </c>
+    </row>
+    <row r="10" spans="1:7" x14ac:dyDescent="0.45">
+      <c r="A10">
+        <v>3.16</v>
+      </c>
+      <c r="B10" s="1">
+        <v>6480</v>
+      </c>
+      <c r="C10">
+        <v>2.84</v>
+      </c>
+      <c r="D10" s="1">
+        <v>1.56E-5</v>
+      </c>
+      <c r="E10">
+        <f t="shared" si="0"/>
+        <v>36.391680000000001</v>
+      </c>
+    </row>
+    <row r="11" spans="1:7" x14ac:dyDescent="0.45">
+      <c r="A11">
+        <v>3.16</v>
+      </c>
+      <c r="B11" s="1">
+        <v>12780</v>
+      </c>
+      <c r="C11">
+        <v>2.2000000000000002</v>
+      </c>
+      <c r="D11" s="1">
+        <v>1.4E-5</v>
+      </c>
+      <c r="E11">
+        <f t="shared" ref="E11:E16" si="1">D11*B11*360</f>
+        <v>64.411199999999994</v>
+      </c>
+    </row>
+    <row r="12" spans="1:7" x14ac:dyDescent="0.45">
+      <c r="A12">
+        <v>3.16</v>
+      </c>
+      <c r="B12" s="1">
+        <v>18070</v>
+      </c>
+      <c r="C12">
+        <v>1.68</v>
+      </c>
+      <c r="D12" s="1">
+        <v>1.29E-5</v>
+      </c>
+      <c r="E12">
+        <f t="shared" si="1"/>
+        <v>83.917079999999999</v>
+      </c>
+    </row>
+    <row r="13" spans="1:7" x14ac:dyDescent="0.45">
+      <c r="A13">
+        <v>3.16</v>
+      </c>
+      <c r="B13" s="1">
+        <v>22500</v>
+      </c>
+      <c r="C13">
+        <v>1.3</v>
+      </c>
+      <c r="D13" s="1">
+        <v>1.1600000000000001E-5</v>
+      </c>
+      <c r="E13">
+        <f t="shared" si="1"/>
+        <v>93.960000000000008</v>
+      </c>
+    </row>
+    <row r="14" spans="1:7" x14ac:dyDescent="0.45">
+      <c r="A14">
+        <v>3.16</v>
+      </c>
+      <c r="B14" s="1">
+        <v>30000</v>
+      </c>
+      <c r="C14" s="1">
+        <v>0.84</v>
+      </c>
+      <c r="D14" s="1">
+        <v>1.08E-5</v>
+      </c>
+      <c r="E14">
+        <f t="shared" si="1"/>
+        <v>116.64</v>
+      </c>
+    </row>
+    <row r="15" spans="1:7" x14ac:dyDescent="0.45">
+      <c r="A15">
+        <v>2.82</v>
+      </c>
+      <c r="B15" s="1">
+        <v>38100</v>
+      </c>
+      <c r="C15" s="1">
+        <v>0.52800000000000002</v>
+      </c>
+      <c r="D15" s="1">
+        <v>9.0000000000000002E-6</v>
+      </c>
+      <c r="E15">
+        <f t="shared" si="1"/>
+        <v>123.44399999999999</v>
+      </c>
+    </row>
+    <row r="16" spans="1:7" x14ac:dyDescent="0.45">
+      <c r="A16">
+        <v>2.78</v>
+      </c>
+      <c r="B16" s="1">
+        <v>50000</v>
+      </c>
+      <c r="C16" s="1">
+        <v>0.3</v>
+      </c>
+      <c r="D16" s="1">
+        <v>8.2800000000000003E-6</v>
+      </c>
+      <c r="E16">
+        <f t="shared" si="1"/>
+        <v>149.04000000000002</v>
+      </c>
+    </row>
+    <row r="17" spans="1:7" x14ac:dyDescent="0.45">
+      <c r="A17" s="1">
+        <v>0.27600000000000002</v>
+      </c>
+      <c r="B17" s="1">
+        <v>57070</v>
+      </c>
+      <c r="C17" s="1">
+        <v>2.52E-2</v>
+      </c>
+      <c r="D17" s="1"/>
+      <c r="E17">
+        <f>180-ASIN(G17/F17)</f>
+        <v>179.34558443775083</v>
+      </c>
+      <c r="F17" s="1">
+        <v>0.28749999999999998</v>
+      </c>
+      <c r="G17">
+        <v>0.17499999999999999</v>
+      </c>
+    </row>
+    <row r="18" spans="1:7" x14ac:dyDescent="0.45">
+      <c r="A18" s="1">
+        <v>2.7399999999999998E-3</v>
+      </c>
+      <c r="B18" s="1">
+        <v>80000</v>
+      </c>
+      <c r="C18" s="1">
+        <v>1.26E-2</v>
+      </c>
+      <c r="E18">
+        <f>180-ASIN(G18/F18)</f>
+        <v>179.8393093470481</v>
+      </c>
+      <c r="F18" s="1">
+        <v>0.2</v>
+      </c>
+      <c r="G18">
+        <v>3.2000000000000001E-2</v>
+      </c>
+    </row>
+    <row r="19" spans="1:7" x14ac:dyDescent="0.45">
+      <c r="A19" s="1">
+        <v>0.16500000000000001</v>
+      </c>
+      <c r="B19" s="1">
+        <v>191100</v>
+      </c>
+      <c r="C19" s="1">
+        <v>1.7600000000000001E-2</v>
+      </c>
+      <c r="E19" s="1">
+        <f>180-ASIN(G19/F19)</f>
+        <v>180</v>
+      </c>
+      <c r="F19" s="1">
+        <v>1</v>
+      </c>
+      <c r="G19">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="20" spans="1:7" x14ac:dyDescent="0.45">
+      <c r="A20" s="1">
+        <v>0.16700000000000001</v>
+      </c>
+      <c r="B20" s="1">
+        <v>1000000</v>
+      </c>
+      <c r="C20" s="1">
+        <v>6.4799999999999996E-2</v>
+      </c>
+      <c r="E20">
+        <f>ASIN(G20/F20)</f>
+        <v>0.6465165714340122</v>
+      </c>
+      <c r="F20" s="1">
+        <v>8.3000000000000007</v>
+      </c>
+      <c r="G20">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="21" spans="1:7" x14ac:dyDescent="0.45">
+      <c r="A21" s="1">
+        <v>0.17</v>
+      </c>
+      <c r="B21" s="1">
+        <v>2700000</v>
+      </c>
+      <c r="C21" s="1">
+        <v>0.08</v>
+      </c>
+      <c r="E21">
+        <f>ASIN(G21/F21)</f>
+        <v>0.18936501004440615</v>
+      </c>
+      <c r="F21" s="1">
+        <v>8.5</v>
+      </c>
+      <c r="G21">
         <v>1.6</v>
-      </c>
-      <c r="D8" s="1">
-        <v>1.1E-5</v>
-      </c>
-      <c r="E8">
-        <f t="shared" si="0"/>
-        <v>71.279999999999987</v>
-      </c>
-    </row>
-    <row r="9" spans="1:5" x14ac:dyDescent="0.45">
-      <c r="B9">
-        <v>20000</v>
-      </c>
-      <c r="C9">
-        <v>1.5</v>
-      </c>
-      <c r="D9" s="1">
-        <v>1.06E-5</v>
-      </c>
-      <c r="E9">
-        <f t="shared" si="0"/>
-        <v>76.319999999999993</v>
-      </c>
-    </row>
-    <row r="10" spans="1:5" x14ac:dyDescent="0.45">
-      <c r="B10">
-        <v>25000</v>
-      </c>
-      <c r="C10">
-        <v>1.2</v>
-      </c>
-      <c r="D10" s="1">
-        <v>9.3999999999999998E-6</v>
-      </c>
-      <c r="E10">
-        <f t="shared" si="0"/>
-        <v>84.6</v>
-      </c>
-    </row>
-    <row r="11" spans="1:5" x14ac:dyDescent="0.45">
-      <c r="B11">
-        <v>30000</v>
-      </c>
-      <c r="C11">
-        <v>1</v>
-      </c>
-      <c r="D11" s="1">
-        <v>8.3999999999999992E-6</v>
-      </c>
-      <c r="E11">
-        <f>D11*B11*360</f>
-        <v>90.72</v>
-      </c>
-    </row>
-    <row r="12" spans="1:5" x14ac:dyDescent="0.45">
-      <c r="B12">
-        <v>180000</v>
-      </c>
-      <c r="D12" s="1">
-        <v>3.4999999999999999E-6</v>
-      </c>
-      <c r="E12">
-        <f>D12*B12*360</f>
-        <v>226.8</v>
       </c>
     </row>
   </sheetData>

</xml_diff>